<commit_message>
organizacion de los directorios
</commit_message>
<xml_diff>
--- a/tests/results.xlsx
+++ b/tests/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inpf\Documents\GitHub\TMOPT\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inpf\Documents\GitHub\old\TMOPT_orig\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="pruebas gioconda" sheetId="3" r:id="rId1"/>
-    <sheet name="pruebas abortadas" sheetId="4" r:id="rId2"/>
+    <sheet name="pruebas gioconda (2)" sheetId="5" r:id="rId2"/>
+    <sheet name="pruebas abortadas" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>fitness</t>
   </si>
@@ -126,43 +127,19 @@
     <t>test 16</t>
   </si>
   <si>
-    <t>test 17</t>
-  </si>
-  <si>
-    <t>Prueba 1: más de 8horas y no termina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['poligonProblem.num_shapes'] = 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['poligonProblem.candidates_by_iteration'] = 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['poligonProblem.delta'] = 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['poligonProblem.max_edges'] = 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['poligonProblem.vns_vnd'] = 'vnd'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['initialSolution.lenght'] = 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['initialTabuSearch.max_iterations'] = 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['initialTabuSearch.list_length'] = 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['initialTabuSearch.tolerance'] = 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['generalTabuSearch.max_iterations'] = 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    params_dict['generalTabuSearch.list_length'] = 5</t>
+    <t>Parámetro</t>
+  </si>
+  <si>
+    <t>test 03</t>
+  </si>
+  <si>
+    <t>Columna2</t>
+  </si>
+  <si>
+    <t>Columna3</t>
+  </si>
+  <si>
+    <t>Columna4</t>
   </si>
 </sst>
 </file>
@@ -216,8 +193,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,8 +216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -252,20 +229,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
       <bottom style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,27 +273,70 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="60% - Énfasis4" xfId="1" builtinId="44"/>
+    <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="36">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -386,8 +413,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="34"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -402,26 +429,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:P14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:N14" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <tableColumns count="14">
     <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="5" name="test 04" dataDxfId="14"/>
-    <tableColumn id="8" name="test 07" dataDxfId="13"/>
-    <tableColumn id="9" name="test 08" dataDxfId="12"/>
-    <tableColumn id="2" name="test 01" dataDxfId="11"/>
-    <tableColumn id="6" name="test 05" dataDxfId="10"/>
-    <tableColumn id="7" name="test 06" dataDxfId="9"/>
-    <tableColumn id="10" name="test 09" dataDxfId="8"/>
-    <tableColumn id="12" name="test 10" dataDxfId="7"/>
-    <tableColumn id="13" name="test 11" dataDxfId="6"/>
-    <tableColumn id="14" name="test 12" dataDxfId="5"/>
-    <tableColumn id="4" name="test 13" dataDxfId="4"/>
-    <tableColumn id="15" name="test 14" dataDxfId="3"/>
-    <tableColumn id="16" name="test 15" dataDxfId="2"/>
-    <tableColumn id="17" name="test 16" dataDxfId="1"/>
-    <tableColumn id="11" name="test 17" dataDxfId="0"/>
+    <tableColumn id="5" name="test 04" dataDxfId="31"/>
+    <tableColumn id="8" name="test 07" dataDxfId="30"/>
+    <tableColumn id="9" name="test 08" dataDxfId="29"/>
+    <tableColumn id="2" name="test 01" dataDxfId="28"/>
+    <tableColumn id="6" name="test 05" dataDxfId="27"/>
+    <tableColumn id="7" name="test 06" dataDxfId="26"/>
+    <tableColumn id="10" name="test 09" dataDxfId="25"/>
+    <tableColumn id="12" name="test 10" dataDxfId="24"/>
+    <tableColumn id="13" name="test 11" dataDxfId="23"/>
+    <tableColumn id="14" name="test 12" dataDxfId="22"/>
+    <tableColumn id="17" name="test 16" dataDxfId="21"/>
+    <tableColumn id="16" name="test 15" dataDxfId="20"/>
+    <tableColumn id="4" name="test 13" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla132" displayName="Tabla132" ref="A1:O14" totalsRowShown="0">
+  <tableColumns count="15">
+    <tableColumn id="1" name="Parámetro"/>
+    <tableColumn id="5" name="test 01" dataDxfId="18"/>
+    <tableColumn id="8" name="test 02" dataDxfId="17"/>
+    <tableColumn id="9" name="test 03" dataDxfId="16"/>
+    <tableColumn id="2" name="test 04" dataDxfId="15"/>
+    <tableColumn id="6" name="test 05" dataDxfId="14"/>
+    <tableColumn id="7" name="test 06" dataDxfId="13"/>
+    <tableColumn id="10" name="test 07" dataDxfId="12"/>
+    <tableColumn id="12" name="test 08" dataDxfId="11"/>
+    <tableColumn id="13" name="test 09" dataDxfId="10"/>
+    <tableColumn id="14" name="test 10" dataDxfId="9"/>
+    <tableColumn id="17" name="test 11" dataDxfId="8"/>
+    <tableColumn id="16" name="test 12" dataDxfId="7"/>
+    <tableColumn id="3" name="test 13" dataDxfId="6"/>
+    <tableColumn id="4" name="test 14" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla134" displayName="Tabla134" ref="A1:D12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Columna1"/>
+    <tableColumn id="15" name="Columna2" dataDxfId="2"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="0"/>
+    <tableColumn id="2" name="Columna4" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -690,14 +750,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="5" max="5" width="11.42578125" style="1"/>
     <col min="8" max="8" width="11.42578125" style="1"/>
     <col min="16" max="16" width="11.42578125" style="1"/>
@@ -739,23 +800,18 @@
         <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="P1"/>
       <c r="R1"/>
       <c r="S1"/>
       <c r="T1"/>
@@ -799,19 +855,18 @@
         <v>27988.23</v>
       </c>
       <c r="L2" s="2">
+        <v>1442.44</v>
+      </c>
+      <c r="M2" s="2">
+        <v>36170.85</v>
+      </c>
+      <c r="N2" s="2">
         <v>6578.67</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2">
-        <v>36170.85</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1442.44</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="6">
+      <c r="O2" s="6">
         <v>17588.98</v>
       </c>
+      <c r="P2"/>
       <c r="R2"/>
       <c r="S2"/>
       <c r="T2"/>
@@ -855,19 +910,18 @@
         <v>33.802300000000002</v>
       </c>
       <c r="L3" s="4">
+        <v>31.466000000000001</v>
+      </c>
+      <c r="M3" s="4">
+        <v>25.376999999999999</v>
+      </c>
+      <c r="N3" s="4">
         <v>23.711099999999998</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4">
-        <v>25.376999999999999</v>
-      </c>
       <c r="O3" s="4">
-        <v>31.466000000000001</v>
-      </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4">
         <v>8.5696999999999992</v>
       </c>
+      <c r="P3"/>
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
@@ -919,15 +973,10 @@
       <c r="N4" s="1">
         <v>5</v>
       </c>
-      <c r="O4" s="1">
-        <v>5</v>
-      </c>
-      <c r="P4" s="1">
+      <c r="O4" s="8">
         <v>100</v>
       </c>
-      <c r="Q4" s="8">
-        <v>100</v>
-      </c>
+      <c r="P4"/>
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
@@ -979,15 +1028,10 @@
       <c r="N5" s="1">
         <v>7</v>
       </c>
-      <c r="O5" s="1">
-        <v>7</v>
-      </c>
-      <c r="P5" s="1">
+      <c r="O5" s="8">
         <v>100</v>
       </c>
-      <c r="Q5" s="8">
-        <v>100</v>
-      </c>
+      <c r="P5"/>
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
@@ -1033,21 +1077,16 @@
       <c r="L6" s="1">
         <v>25</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="1">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1">
+        <v>25</v>
+      </c>
+      <c r="O6" s="8">
         <v>100</v>
       </c>
-      <c r="N6" s="1">
-        <v>25</v>
-      </c>
-      <c r="O6" s="1">
-        <v>25</v>
-      </c>
-      <c r="P6" s="1">
-        <v>100</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>100</v>
-      </c>
+      <c r="P6"/>
       <c r="R6"/>
       <c r="S6"/>
       <c r="T6"/>
@@ -1099,15 +1138,10 @@
       <c r="N7" s="1">
         <v>2</v>
       </c>
-      <c r="O7" s="1">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>2</v>
-      </c>
+      <c r="O7" s="6">
+        <v>2</v>
+      </c>
+      <c r="P7"/>
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
@@ -1153,21 +1187,16 @@
       <c r="L8" s="1">
         <v>7</v>
       </c>
-      <c r="M8" s="1">
-        <v>7</v>
-      </c>
-      <c r="N8" s="7">
-        <v>25</v>
-      </c>
-      <c r="O8" s="1">
-        <v>7</v>
-      </c>
-      <c r="P8" s="1">
+      <c r="M8" s="7">
+        <v>25</v>
+      </c>
+      <c r="N8" s="1">
+        <v>7</v>
+      </c>
+      <c r="O8" s="8">
         <v>100</v>
       </c>
-      <c r="Q8" s="8">
-        <v>100</v>
-      </c>
+      <c r="P8"/>
       <c r="R8"/>
       <c r="S8"/>
       <c r="T8"/>
@@ -1210,8 +1239,8 @@
       <c r="K9" s="1">
         <v>50</v>
       </c>
-      <c r="L9" s="1">
-        <v>50</v>
+      <c r="L9" s="7">
+        <v>100</v>
       </c>
       <c r="M9" s="1">
         <v>50</v>
@@ -1219,15 +1248,10 @@
       <c r="N9" s="1">
         <v>50</v>
       </c>
-      <c r="O9" s="7">
-        <v>100</v>
-      </c>
-      <c r="P9" s="1">
-        <v>50</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>50</v>
-      </c>
+      <c r="O9" s="6">
+        <v>50</v>
+      </c>
+      <c r="P9"/>
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -1270,24 +1294,19 @@
       <c r="K10" s="1">
         <v>3</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <v>3</v>
+      </c>
+      <c r="N10" s="7">
         <v>6</v>
       </c>
-      <c r="M10" s="1">
-        <v>3</v>
-      </c>
-      <c r="N10" s="1">
-        <v>3</v>
-      </c>
-      <c r="O10" s="1">
-        <v>3</v>
-      </c>
-      <c r="P10" s="1">
+      <c r="O10" s="8">
         <v>100</v>
       </c>
-      <c r="Q10" s="8">
-        <v>100</v>
-      </c>
+      <c r="P10"/>
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -1339,15 +1358,10 @@
       <c r="N11" s="1">
         <v>50</v>
       </c>
-      <c r="O11" s="1">
-        <v>50</v>
-      </c>
-      <c r="P11" s="1">
-        <v>50</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>50</v>
-      </c>
+      <c r="O11" s="6">
+        <v>50</v>
+      </c>
+      <c r="P11"/>
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -1399,15 +1413,10 @@
       <c r="N12" s="1">
         <v>4</v>
       </c>
-      <c r="O12" s="1">
-        <v>4</v>
-      </c>
-      <c r="P12" s="7">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>7</v>
-      </c>
+      <c r="O12" s="8">
+        <v>7</v>
+      </c>
+      <c r="P12"/>
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>
@@ -1459,15 +1468,10 @@
       <c r="N13" s="1">
         <v>1</v>
       </c>
-      <c r="O13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>1</v>
-      </c>
+      <c r="O13" s="6">
+        <v>1</v>
+      </c>
+      <c r="P13"/>
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
@@ -1519,15 +1523,10 @@
       <c r="N14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="1" t="s">
+      <c r="O14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="P14"/>
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
@@ -1547,167 +1546,1106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
+    <col min="8" max="10" width="9" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1"/>
+    <col min="18" max="24" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>28.85</v>
+      </c>
+      <c r="D2" s="1">
+        <v>93.53</v>
+      </c>
+      <c r="E2" s="1">
+        <v>228.63</v>
+      </c>
+      <c r="F2" s="1">
+        <v>166.15</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1557.75</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3291.54</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1665.63</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1093.57</v>
+      </c>
+      <c r="K2" s="1">
+        <v>27988.23</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1442.44</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36170.85</v>
+      </c>
+      <c r="N2" s="1">
+        <v>6578.67</v>
+      </c>
+      <c r="O2" s="1">
+        <v>17588.98</v>
+      </c>
+      <c r="P2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>600.49969999999996</v>
+      </c>
+      <c r="C3" s="2">
+        <v>319.45339999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>248.84289999999999</v>
+      </c>
+      <c r="E3" s="2">
+        <v>189.01070000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>50.828400000000002</v>
+      </c>
+      <c r="G3" s="2">
+        <v>34.846800000000002</v>
+      </c>
+      <c r="H3" s="2">
+        <v>31.7941</v>
+      </c>
+      <c r="I3" s="2">
+        <v>35.867100000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>32.346699999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>33.802300000000002</v>
+      </c>
+      <c r="L3" s="2">
+        <v>31.466000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>25.376999999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>23.711099999999998</v>
+      </c>
+      <c r="O3" s="9">
+        <v>8.5696999999999992</v>
+      </c>
+      <c r="P3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1">
+        <v>100</v>
+      </c>
+      <c r="P4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1">
+        <v>7</v>
+      </c>
+      <c r="L5" s="1">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1">
+        <v>7</v>
+      </c>
+      <c r="N5" s="1">
+        <v>7</v>
+      </c>
+      <c r="O5" s="1">
+        <v>100</v>
+      </c>
+      <c r="P5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1">
+        <v>25</v>
+      </c>
+      <c r="O6" s="1">
+        <v>100</v>
+      </c>
+      <c r="P6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>2</v>
+      </c>
+      <c r="P7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7</v>
+      </c>
+      <c r="L8" s="1">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1">
+        <v>25</v>
+      </c>
+      <c r="N8" s="1">
+        <v>7</v>
+      </c>
+      <c r="O8" s="1">
+        <v>100</v>
+      </c>
+      <c r="P8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1">
+        <v>50</v>
+      </c>
+      <c r="J9" s="1">
+        <v>50</v>
+      </c>
+      <c r="K9" s="1">
+        <v>50</v>
+      </c>
+      <c r="L9" s="1">
+        <v>100</v>
+      </c>
+      <c r="M9" s="1">
+        <v>50</v>
+      </c>
+      <c r="N9" s="1">
+        <v>50</v>
+      </c>
+      <c r="O9" s="1">
+        <v>50</v>
+      </c>
+      <c r="P9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>3</v>
+      </c>
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <v>3</v>
+      </c>
+      <c r="N10" s="1">
+        <v>6</v>
+      </c>
+      <c r="O10" s="1">
+        <v>100</v>
+      </c>
+      <c r="P10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1">
+        <v>50</v>
+      </c>
+      <c r="J11" s="1">
+        <v>50</v>
+      </c>
+      <c r="K11" s="1">
+        <v>50</v>
+      </c>
+      <c r="L11" s="1">
+        <v>50</v>
+      </c>
+      <c r="M11" s="1">
+        <v>50</v>
+      </c>
+      <c r="N11" s="1">
+        <v>50</v>
+      </c>
+      <c r="O11" s="1">
+        <v>50</v>
+      </c>
+      <c r="P11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>4</v>
+      </c>
+      <c r="L12" s="1">
+        <v>4</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1">
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <v>7</v>
+      </c>
+      <c r="P12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>5</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <v>7</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>25</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
-        <v>2</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>7</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
-        <v>50</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>25</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <v>50</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>4</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <v>1</v>
-      </c>
-      <c r="B27" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1</v>
+      </c>
+      <c r="P13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="11" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>75</v>
+      </c>
+      <c r="C4" s="10">
+        <v>50</v>
+      </c>
+      <c r="D4" s="10">
+        <v>25</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1">
+        <v>50</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>